<commit_message>
Nouveaux ajouts sur sous branche LAVOTTE-ALLEGRAUD
</commit_message>
<xml_diff>
--- a/Famille/Global.xlsx
+++ b/Famille/Global.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zinaon\git\Genealogie\Famille\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D631AA-CD3B-4B98-8863-D05BA445E8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFBB51E-CC66-4511-BFD6-7C80CCA02FFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{0B8BDED2-C876-4219-A4EE-2B98E8105897}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="443">
   <si>
     <t>N°</t>
   </si>
@@ -801,9 +801,6 @@
     <t>22/05/1864</t>
   </si>
   <si>
-    <t>02/01/1848</t>
-  </si>
-  <si>
     <t>Saint Junien</t>
   </si>
   <si>
@@ -1300,6 +1297,75 @@
   </si>
   <si>
     <t>Louise</t>
+  </si>
+  <si>
+    <t>27/01/1848</t>
+  </si>
+  <si>
+    <t>16/10/1831</t>
+  </si>
+  <si>
+    <t>10/10/1810</t>
+  </si>
+  <si>
+    <t>07/02/1826</t>
+  </si>
+  <si>
+    <t>Saint-Victurnien</t>
+  </si>
+  <si>
+    <t>LAVOUTTE</t>
+  </si>
+  <si>
+    <t>25/10/1811</t>
+  </si>
+  <si>
+    <t>ALLEGRAUD</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>VARIELLE</t>
+  </si>
+  <si>
+    <t>Cognac la forêt</t>
+  </si>
+  <si>
+    <t>TROUTAUD</t>
+  </si>
+  <si>
+    <t>Cognac la foret</t>
+  </si>
+  <si>
+    <t>24/01/1809</t>
+  </si>
+  <si>
+    <t>24/04/1788</t>
+  </si>
+  <si>
+    <t>03/10/1788</t>
+  </si>
+  <si>
+    <t>PECHE</t>
+  </si>
+  <si>
+    <t>13/10/1820</t>
+  </si>
+  <si>
+    <t>16/01/1824</t>
+  </si>
+  <si>
+    <t>03/01/1832</t>
+  </si>
+  <si>
+    <t>30/06/1832</t>
+  </si>
+  <si>
+    <t>15/07/1825</t>
+  </si>
+  <si>
+    <t>26/01/1829</t>
   </si>
 </sst>
 </file>
@@ -1424,12 +1490,12 @@
     <tableColumn id="5" xr3:uid="{7012F2EB-5A9B-4C4E-ADEE-C5153B236B8B}" name="Lieu naissance"/>
     <tableColumn id="6" xr3:uid="{AC0B7C6F-39E5-44DA-A983-E0ADD53C9978}" name="Date mariage"/>
     <tableColumn id="7" xr3:uid="{319B3D1D-1C51-4654-9129-454B0D846915}" name="Lieu mariage"/>
-    <tableColumn id="11" xr3:uid="{94319078-F8E6-4DD9-90DA-CCF2559C57A9}" name="Date décès" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{94319078-F8E6-4DD9-90DA-CCF2559C57A9}" name="Date décès" dataDxfId="4"/>
     <tableColumn id="12" xr3:uid="{6452005E-B0B8-4910-9A60-CBF6A33A3ED9}" name="Lieu décès"/>
-    <tableColumn id="9" xr3:uid="{E37C3C5C-A389-4882-95CA-79A8C3730025}" name="N° Père" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{E37C3C5C-A389-4882-95CA-79A8C3730025}" name="N° Père" dataDxfId="3">
       <calculatedColumnFormula>Tableau13[[#This Row],[N°]]*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{4AD1E9DB-87A6-47DE-BBAA-FD68AD38B0D2}" name="N°Mère" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{4AD1E9DB-87A6-47DE-BBAA-FD68AD38B0D2}" name="N°Mère" dataDxfId="2">
       <calculatedColumnFormula>Tableau13[[#This Row],[N°]]*2+1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4473,10 +4539,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C738DB9D-15CD-457A-B92C-674AA9158BB4}">
-  <dimension ref="A1:K161"/>
+  <dimension ref="A1:P161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="L24:O24"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="N88" sqref="N88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4780,10 +4846,10 @@
         <v>47</v>
       </c>
       <c r="D11" t="s">
+        <v>420</v>
+      </c>
+      <c r="E11" t="s">
         <v>254</v>
-      </c>
-      <c r="E11" t="s">
-        <v>255</v>
       </c>
       <c r="J11">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -4805,16 +4871,16 @@
         <v>49</v>
       </c>
       <c r="D12" t="s">
+        <v>255</v>
+      </c>
+      <c r="E12" t="s">
         <v>256</v>
-      </c>
-      <c r="E12" t="s">
-        <v>257</v>
       </c>
       <c r="H12" s="2">
         <v>5280</v>
       </c>
       <c r="I12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J12">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -4833,19 +4899,19 @@
         <v>205</v>
       </c>
       <c r="C13" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" t="s">
         <v>258</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>259</v>
-      </c>
-      <c r="E13" t="s">
-        <v>260</v>
       </c>
       <c r="H13" s="2">
         <v>12435</v>
       </c>
       <c r="I13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J13">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -4864,16 +4930,16 @@
         <v>202</v>
       </c>
       <c r="C14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D14" t="s">
         <v>262</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>263</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>264</v>
-      </c>
-      <c r="H14" t="s">
-        <v>265</v>
       </c>
       <c r="I14" t="s">
         <v>247</v>
@@ -4898,10 +4964,10 @@
         <v>181</v>
       </c>
       <c r="D15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E15" t="s">
         <v>266</v>
-      </c>
-      <c r="E15" t="s">
-        <v>267</v>
       </c>
       <c r="J15">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -4920,16 +4986,16 @@
         <v>199</v>
       </c>
       <c r="C16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" t="s">
         <v>268</v>
-      </c>
-      <c r="D16" t="s">
-        <v>269</v>
       </c>
       <c r="E16" t="s">
         <v>240</v>
       </c>
       <c r="F16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J16">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -4951,7 +5017,7 @@
         <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E17" t="s">
         <v>233</v>
@@ -4976,13 +5042,13 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
+        <v>271</v>
+      </c>
+      <c r="E18" t="s">
         <v>272</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>273</v>
-      </c>
-      <c r="F18" t="s">
-        <v>274</v>
       </c>
       <c r="G18" t="s">
         <v>240</v>
@@ -5007,7 +5073,7 @@
         <v>181</v>
       </c>
       <c r="D19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E19" t="s">
         <v>240</v>
@@ -5032,13 +5098,13 @@
         <v>238</v>
       </c>
       <c r="D20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E20" t="s">
         <v>240</v>
       </c>
       <c r="H20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I20" t="s">
         <v>233</v>
@@ -5060,16 +5126,16 @@
         <v>209</v>
       </c>
       <c r="C21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" t="s">
         <v>278</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>279</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>280</v>
-      </c>
-      <c r="H21" t="s">
-        <v>281</v>
       </c>
       <c r="I21" t="s">
         <v>233</v>
@@ -5093,8 +5159,17 @@
       <c r="C22" t="s">
         <v>89</v>
       </c>
-      <c r="D22">
-        <v>1812</v>
+      <c r="D22" t="s">
+        <v>422</v>
+      </c>
+      <c r="E22" t="s">
+        <v>432</v>
+      </c>
+      <c r="F22" t="s">
+        <v>421</v>
+      </c>
+      <c r="G22" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -5107,6 +5182,12 @@
       <c r="C23" t="s">
         <v>47</v>
       </c>
+      <c r="D23" t="s">
+        <v>426</v>
+      </c>
+      <c r="E23" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -5119,10 +5200,10 @@
         <v>89</v>
       </c>
       <c r="D24" t="s">
+        <v>416</v>
+      </c>
+      <c r="E24" t="s">
         <v>417</v>
-      </c>
-      <c r="E24" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -5133,7 +5214,7 @@
         <v>211</v>
       </c>
       <c r="C25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5147,16 +5228,16 @@
         <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G26" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -5170,10 +5251,10 @@
         <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J27">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5195,16 +5276,16 @@
         <v>97</v>
       </c>
       <c r="D28" t="s">
+        <v>283</v>
+      </c>
+      <c r="E28" t="s">
+        <v>263</v>
+      </c>
+      <c r="F28" t="s">
         <v>284</v>
       </c>
-      <c r="E28" t="s">
-        <v>264</v>
-      </c>
-      <c r="F28" t="s">
-        <v>285</v>
-      </c>
       <c r="G28" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J28">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5226,10 +5307,10 @@
         <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J29">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5259,7 +5340,7 @@
         <v>214</v>
       </c>
       <c r="C31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -5276,10 +5357,10 @@
         <v>240</v>
       </c>
       <c r="F32" t="s">
+        <v>287</v>
+      </c>
+      <c r="H32" t="s">
         <v>288</v>
-      </c>
-      <c r="H32" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -5310,7 +5391,7 @@
         <v>233</v>
       </c>
       <c r="H34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I34" t="s">
         <v>233</v>
@@ -5335,10 +5416,10 @@
         <v>203</v>
       </c>
       <c r="C36" t="s">
+        <v>290</v>
+      </c>
+      <c r="H36" t="s">
         <v>291</v>
-      </c>
-      <c r="H36" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -5352,7 +5433,7 @@
         <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I37" t="s">
         <v>240</v>
@@ -5369,7 +5450,7 @@
         <v>49</v>
       </c>
       <c r="H38" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I38" t="s">
         <v>242</v>
@@ -5380,13 +5461,13 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
+        <v>294</v>
+      </c>
+      <c r="C39" t="s">
         <v>295</v>
       </c>
-      <c r="C39" t="s">
+      <c r="H39" t="s">
         <v>296</v>
-      </c>
-      <c r="H39" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -5400,10 +5481,10 @@
         <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E40" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J40">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5425,10 +5506,10 @@
         <v>47</v>
       </c>
       <c r="H41" t="s">
+        <v>298</v>
+      </c>
+      <c r="I41" t="s">
         <v>299</v>
-      </c>
-      <c r="I41" t="s">
-        <v>300</v>
       </c>
       <c r="J41">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5450,7 +5531,7 @@
         <v>231</v>
       </c>
       <c r="D42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E42" t="s">
         <v>242</v>
@@ -5472,10 +5553,10 @@
         <v>219</v>
       </c>
       <c r="C43" t="s">
+        <v>301</v>
+      </c>
+      <c r="D43" t="s">
         <v>302</v>
-      </c>
-      <c r="D43" t="s">
-        <v>303</v>
       </c>
       <c r="E43" t="s">
         <v>233</v>
@@ -5489,6 +5570,90 @@
         <v>87</v>
       </c>
     </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>425</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" t="s">
+        <v>434</v>
+      </c>
+      <c r="E44" t="s">
+        <v>432</v>
+      </c>
+      <c r="F44" t="s">
+        <v>433</v>
+      </c>
+      <c r="G44" t="s">
+        <v>430</v>
+      </c>
+      <c r="J44">
+        <f>Tableau14[[#This Row],[N°]]*2</f>
+        <v>88</v>
+      </c>
+      <c r="K44">
+        <f>Tableau14[[#This Row],[N° Père]]+1</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>431</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>435</v>
+      </c>
+      <c r="E45" t="s">
+        <v>432</v>
+      </c>
+      <c r="H45" t="s">
+        <v>423</v>
+      </c>
+      <c r="I45" t="s">
+        <v>430</v>
+      </c>
+      <c r="J45">
+        <f>Tableau14[[#This Row],[N°]]*2</f>
+        <v>90</v>
+      </c>
+      <c r="K45">
+        <f>Tableau14[[#This Row],[N° Père]]+1</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>427</v>
+      </c>
+      <c r="C46" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>429</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>48</v>
@@ -5505,10 +5670,10 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
+        <v>418</v>
+      </c>
+      <c r="C49" t="s">
         <v>419</v>
-      </c>
-      <c r="C49" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5550,10 +5715,10 @@
         <v>1760</v>
       </c>
       <c r="H56" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I56" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -5570,10 +5735,10 @@
         <v>1762</v>
       </c>
       <c r="H57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I57" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -5590,10 +5755,10 @@
         <v>1770</v>
       </c>
       <c r="H58" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -5604,19 +5769,19 @@
         <v>222</v>
       </c>
       <c r="C59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D59">
         <v>1768</v>
       </c>
       <c r="E59" t="s">
+        <v>307</v>
+      </c>
+      <c r="H59" t="s">
         <v>308</v>
       </c>
-      <c r="H59" t="s">
-        <v>309</v>
-      </c>
       <c r="I59" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -5627,7 +5792,7 @@
         <v>201</v>
       </c>
       <c r="C80" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J80">
         <f>Tableau14[[#This Row],[N°]]*2</f>
@@ -5638,7 +5803,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>81</v>
       </c>
@@ -5649,7 +5814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>82</v>
       </c>
@@ -5660,7 +5825,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>83</v>
       </c>
@@ -5671,7 +5836,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>84</v>
       </c>
@@ -5682,18 +5847,18 @@
         <v>238</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C85" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>86</v>
       </c>
@@ -5704,7 +5869,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>87</v>
       </c>
@@ -5713,6 +5878,68 @@
       </c>
       <c r="C87" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>204</v>
+      </c>
+      <c r="C88" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>436</v>
+      </c>
+      <c r="C89" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>431</v>
+      </c>
+      <c r="C90" t="s">
+        <v>89</v>
+      </c>
+      <c r="M90" t="s">
+        <v>437</v>
+      </c>
+      <c r="N90" t="s">
+        <v>438</v>
+      </c>
+      <c r="O90" t="s">
+        <v>439</v>
+      </c>
+      <c r="P90" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>322</v>
+      </c>
+      <c r="C91" t="s">
+        <v>82</v>
+      </c>
+      <c r="M91" t="s">
+        <v>441</v>
+      </c>
+      <c r="N91" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -5811,7 +6038,7 @@
         <v>201</v>
       </c>
       <c r="C160" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -5822,10 +6049,10 @@
         <v>230</v>
       </c>
       <c r="C161" t="s">
+        <v>312</v>
+      </c>
+      <c r="H161" t="s">
         <v>313</v>
-      </c>
-      <c r="H161" t="s">
-        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5896,16 +6123,16 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" t="s">
         <v>338</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>339</v>
-      </c>
-      <c r="E2" t="s">
-        <v>340</v>
       </c>
       <c r="F2" s="1">
         <v>6645</v>
@@ -5925,13 +6152,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" t="s">
         <v>341</v>
-      </c>
-      <c r="D3" t="s">
-        <v>342</v>
       </c>
       <c r="E3" t="s">
         <v>234</v>
@@ -5942,19 +6169,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4" t="s">
         <v>343</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>344</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>345</v>
-      </c>
-      <c r="F4" t="s">
-        <v>346</v>
       </c>
       <c r="G4" t="s">
         <v>234</v>
@@ -5965,16 +6192,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C5" t="s">
         <v>53</v>
       </c>
       <c r="D5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E5" t="s">
         <v>347</v>
-      </c>
-      <c r="E5" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5982,22 +6209,22 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>348</v>
+      </c>
+      <c r="C6" t="s">
         <v>349</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>350</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>351</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>352</v>
       </c>
-      <c r="F6" t="s">
-        <v>353</v>
-      </c>
       <c r="G6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -6005,16 +6232,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C7" t="s">
         <v>181</v>
       </c>
       <c r="D7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -6022,28 +6249,28 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C8" t="s">
+        <v>354</v>
+      </c>
+      <c r="D8" t="s">
         <v>355</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>356</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>357</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>344</v>
+      </c>
+      <c r="H8" t="s">
         <v>358</v>
       </c>
-      <c r="G8" t="s">
-        <v>345</v>
-      </c>
-      <c r="H8" t="s">
-        <v>359</v>
-      </c>
       <c r="I8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -6051,22 +6278,22 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C9" t="s">
         <v>85</v>
       </c>
       <c r="D9" t="s">
+        <v>359</v>
+      </c>
+      <c r="E9" t="s">
+        <v>344</v>
+      </c>
+      <c r="H9" t="s">
         <v>360</v>
       </c>
-      <c r="E9" t="s">
-        <v>345</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>361</v>
-      </c>
-      <c r="I9" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -6074,19 +6301,19 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C10" t="s">
         <v>93</v>
       </c>
       <c r="D10" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" t="s">
         <v>363</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>364</v>
-      </c>
-      <c r="F10" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -6094,16 +6321,16 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
       </c>
       <c r="D11" t="s">
+        <v>365</v>
+      </c>
+      <c r="E11" t="s">
         <v>366</v>
-      </c>
-      <c r="E11" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -6111,28 +6338,28 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C12" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" t="s">
         <v>368</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>369</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G12" t="s">
+        <v>351</v>
+      </c>
+      <c r="H12" t="s">
         <v>370</v>
       </c>
-      <c r="F12" t="s">
-        <v>374</v>
-      </c>
-      <c r="G12" t="s">
-        <v>352</v>
-      </c>
-      <c r="H12" t="s">
-        <v>371</v>
-      </c>
       <c r="I12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -6140,22 +6367,22 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C13" t="s">
         <v>96</v>
       </c>
       <c r="D13" t="s">
+        <v>371</v>
+      </c>
+      <c r="E13" t="s">
         <v>372</v>
       </c>
-      <c r="E13" t="s">
-        <v>373</v>
-      </c>
       <c r="H13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -6163,28 +6390,28 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D14" t="s">
         <v>378</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>375</v>
+      </c>
+      <c r="F14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" t="s">
+        <v>375</v>
+      </c>
+      <c r="H14" t="s">
         <v>379</v>
       </c>
-      <c r="E14" t="s">
-        <v>376</v>
-      </c>
-      <c r="F14" t="s">
-        <v>377</v>
-      </c>
-      <c r="G14" t="s">
-        <v>376</v>
-      </c>
-      <c r="H14" t="s">
-        <v>380</v>
-      </c>
       <c r="I14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -6192,21 +6419,21 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C15" t="s">
         <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -6214,16 +6441,16 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D17" t="s">
+        <v>381</v>
+      </c>
+      <c r="E17" t="s">
         <v>382</v>
-      </c>
-      <c r="E17" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6231,22 +6458,22 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C18" t="s">
+        <v>383</v>
+      </c>
+      <c r="D18" t="s">
         <v>384</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>385</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>386</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>387</v>
-      </c>
-      <c r="G18" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -6254,16 +6481,16 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C19" t="s">
         <v>47</v>
       </c>
       <c r="D19" t="s">
+        <v>388</v>
+      </c>
+      <c r="E19" t="s">
         <v>389</v>
-      </c>
-      <c r="E19" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -6271,7 +6498,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C20" t="s">
         <v>93</v>
@@ -6285,10 +6512,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -6296,7 +6523,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C22" t="s">
         <v>49</v>
@@ -6310,7 +6537,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
@@ -6321,16 +6548,16 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H24" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -6338,10 +6565,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -6349,22 +6576,22 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C26" t="s">
+        <v>393</v>
+      </c>
+      <c r="D26" t="s">
         <v>394</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>395</v>
       </c>
-      <c r="E26" t="s">
+      <c r="H26" t="s">
         <v>396</v>
       </c>
-      <c r="H26" t="s">
-        <v>397</v>
-      </c>
       <c r="I26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6372,22 +6599,22 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C27" t="s">
         <v>82</v>
       </c>
       <c r="D27" t="s">
+        <v>397</v>
+      </c>
+      <c r="E27" t="s">
+        <v>372</v>
+      </c>
+      <c r="H27" t="s">
         <v>398</v>
       </c>
-      <c r="E27" t="s">
-        <v>373</v>
-      </c>
-      <c r="H27" t="s">
-        <v>399</v>
-      </c>
       <c r="I27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6395,7 +6622,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C28" t="s">
         <v>49</v>
@@ -6404,10 +6631,10 @@
         <v>1774</v>
       </c>
       <c r="H28" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6415,16 +6642,16 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
       </c>
       <c r="H29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I29" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -6432,7 +6659,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C30" t="s">
         <v>89</v>
@@ -6441,10 +6668,10 @@
         <v>1762</v>
       </c>
       <c r="H30" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -6452,26 +6679,26 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C31" t="s">
         <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -6479,7 +6706,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C34" t="s">
         <v>93</v>
@@ -6490,10 +6717,10 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -6501,7 +6728,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C36" t="s">
         <v>97</v>
@@ -6512,10 +6739,10 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C37" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -6523,19 +6750,19 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C38" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E38" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H38" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -6543,13 +6770,13 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
       </c>
       <c r="H39" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -6557,7 +6784,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C52" t="s">
         <v>238</v>
@@ -6568,7 +6795,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C53" t="s">
         <v>47</v>
@@ -6579,7 +6806,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C54" t="s">
         <v>89</v>
@@ -6590,7 +6817,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C55" t="s">
         <v>82</v>
@@ -6601,7 +6828,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C56" t="s">
         <v>93</v>
@@ -6612,7 +6839,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C57" t="s">
         <v>181</v>
@@ -6623,7 +6850,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C58" t="s">
         <v>95</v>
@@ -6634,7 +6861,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C59" t="s">
         <v>181</v>
@@ -6645,7 +6872,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C60" t="s">
         <v>97</v>
@@ -6654,10 +6881,10 @@
         <v>1746</v>
       </c>
       <c r="H60" t="s">
+        <v>407</v>
+      </c>
+      <c r="I60" t="s">
         <v>408</v>
-      </c>
-      <c r="I60" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -6665,16 +6892,16 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C61" t="s">
         <v>181</v>
       </c>
       <c r="H61" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I61" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -6682,7 +6909,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C62" t="s">
         <v>49</v>
@@ -6693,19 +6920,19 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C63" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D63">
         <v>1752</v>
       </c>
       <c r="H63" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>